<commit_message>
Updated cost-benefit worksheet. Added Executive recommendation on fuzzing
</commit_message>
<xml_diff>
--- a/Cost-benefit-analysis-worksheet.xlsx
+++ b/Cost-benefit-analysis-worksheet.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="17480" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="33600" windowHeight="17480" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -180,11 +180,11 @@
     <xf numFmtId="44" fontId="2" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="4">
     <cellStyle name="Currency" xfId="1" builtinId="4"/>
@@ -193,60 +193,6 @@
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="9">
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <scheme val="minor"/>
-      </font>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <scheme val="minor"/>
-      </font>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <scheme val="minor"/>
-      </font>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
     <dxf>
       <font>
         <b val="0"/>
@@ -298,6 +244,7 @@
         <name val="Calibri"/>
         <scheme val="minor"/>
       </font>
+      <numFmt numFmtId="0" formatCode="General"/>
     </dxf>
     <dxf>
       <font>
@@ -315,6 +262,59 @@
         <name val="Calibri"/>
         <scheme val="minor"/>
       </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="0" formatCode="General"/>
     </dxf>
     <dxf>
       <font>
@@ -361,7 +361,7 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="B2:F11" dataDxfId="4" dataCellStyle="Currency">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="B2:F11" dataDxfId="8" dataCellStyle="Currency">
   <autoFilter ref="B2:F11">
     <filterColumn colId="0" hiddenButton="1"/>
     <filterColumn colId="1" hiddenButton="1"/>
@@ -371,10 +371,10 @@
   </autoFilter>
   <tableColumns count="5">
     <tableColumn id="1" name=" " totalsRowLabel="Total"/>
-    <tableColumn id="2" name="Sulley" dataDxfId="8" totalsRowDxfId="0" dataCellStyle="Currency"/>
-    <tableColumn id="3" name="Peach_x000a_Community" dataDxfId="7" totalsRowDxfId="1" dataCellStyle="Currency"/>
-    <tableColumn id="4" name="Peach_x000a_Professional" dataDxfId="6" totalsRowDxfId="2" dataCellStyle="Currency"/>
-    <tableColumn id="5" name="Codenomicon" totalsRowFunction="sum" dataDxfId="5" totalsRowDxfId="3" dataCellStyle="Currency"/>
+    <tableColumn id="2" name="Sulley" dataDxfId="7" totalsRowDxfId="6" dataCellStyle="Currency"/>
+    <tableColumn id="3" name="Peach_x000a_Community" dataDxfId="5" totalsRowDxfId="4" dataCellStyle="Currency"/>
+    <tableColumn id="4" name="Peach_x000a_Professional" dataDxfId="3" totalsRowDxfId="2" dataCellStyle="Currency"/>
+    <tableColumn id="5" name="Codenomicon" totalsRowFunction="sum" dataDxfId="1" totalsRowDxfId="0" dataCellStyle="Currency"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium9" showFirstColumn="1" showLastColumn="0" showRowStripes="0" showColumnStripes="1"/>
 </table>
@@ -645,7 +645,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:G21"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="160" zoomScaleNormal="160" zoomScalePageLayoutView="160" workbookViewId="0"/>
+    <sheetView tabSelected="1" zoomScale="160" zoomScaleNormal="160" zoomScalePageLayoutView="160" workbookViewId="0">
+      <selection activeCell="F4" sqref="F4"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
@@ -685,7 +687,7 @@
         <v>5000</v>
       </c>
       <c r="F3" s="1">
-        <v>10000</v>
+        <v>15000</v>
       </c>
     </row>
     <row r="4" spans="2:7" x14ac:dyDescent="0.2">
@@ -727,7 +729,7 @@
       </c>
       <c r="F5" s="1">
         <f>F3*0.2</f>
-        <v>2000</v>
+        <v>3000</v>
       </c>
     </row>
     <row r="6" spans="2:7" x14ac:dyDescent="0.2">
@@ -748,7 +750,7 @@
       </c>
       <c r="F6" s="1">
         <f t="shared" si="0"/>
-        <v>2000</v>
+        <v>3000</v>
       </c>
     </row>
     <row r="7" spans="2:7" x14ac:dyDescent="0.2">
@@ -790,7 +792,7 @@
       </c>
       <c r="F8" s="1">
         <f t="shared" si="1"/>
-        <v>2000</v>
+        <v>3000</v>
       </c>
     </row>
     <row r="9" spans="2:7" x14ac:dyDescent="0.2">
@@ -815,7 +817,7 @@
       </c>
     </row>
     <row r="11" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B11" s="6" t="s">
+      <c r="B11" s="5" t="s">
         <v>3</v>
       </c>
       <c r="C11" s="1">
@@ -832,7 +834,7 @@
       </c>
       <c r="F11" s="1">
         <f>SUM(F3:F10)</f>
-        <v>23250</v>
+        <v>31250</v>
       </c>
     </row>
     <row r="12" spans="2:7" x14ac:dyDescent="0.2">
@@ -842,19 +844,19 @@
       <c r="F12"/>
     </row>
     <row r="14" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B14" s="6" t="s">
+      <c r="B14" s="5" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="15" spans="2:7" ht="35" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B15" s="4" t="s">
+      <c r="B15" s="6" t="s">
         <v>20</v>
       </c>
-      <c r="C15" s="4"/>
-      <c r="D15" s="4"/>
-      <c r="E15" s="4"/>
-      <c r="F15" s="4"/>
-      <c r="G15" s="4"/>
+      <c r="C15" s="6"/>
+      <c r="D15" s="6"/>
+      <c r="E15" s="6"/>
+      <c r="F15" s="6"/>
+      <c r="G15" s="6"/>
     </row>
     <row r="16" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B16" t="s">
@@ -862,14 +864,14 @@
       </c>
     </row>
     <row r="17" spans="2:7" ht="49" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B17" s="4" t="s">
+      <c r="B17" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="C17" s="4"/>
-      <c r="D17" s="4"/>
-      <c r="E17" s="4"/>
-      <c r="F17" s="4"/>
-      <c r="G17" s="4"/>
+      <c r="C17" s="6"/>
+      <c r="D17" s="6"/>
+      <c r="E17" s="6"/>
+      <c r="F17" s="6"/>
+      <c r="G17" s="6"/>
     </row>
     <row r="18" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B18" t="s">
@@ -882,7 +884,7 @@
       </c>
     </row>
     <row r="20" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B20" s="5" t="s">
+      <c r="B20" s="4" t="s">
         <v>17</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Updated Fuzzing and CBA documents and lab notebook
</commit_message>
<xml_diff>
--- a/Cost-benefit-analysis-worksheet.xlsx
+++ b/Cost-benefit-analysis-worksheet.xlsx
@@ -9,10 +9,11 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="33600" windowHeight="17480" tabRatio="500"/>
+    <workbookView xWindow="2080" yWindow="460" windowWidth="25600" windowHeight="17480" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="150000" concurrentCalc="0"/>
   <extLst>
@@ -27,15 +28,12 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="24">
   <si>
     <t>Sulley</t>
   </si>
   <si>
     <t>Codenomicon</t>
-  </si>
-  <si>
-    <t>Implementation - Labor ($50/man-hour)</t>
   </si>
   <si>
     <t>Total Costs</t>
@@ -52,27 +50,15 @@
     <t>Implementation - Licensing (Year 1)</t>
   </si>
   <si>
-    <t>Ongoing Labor (Year 2) ($50/man-hour)</t>
-  </si>
-  <si>
     <t>Software Maintenance (Year 2)</t>
   </si>
   <si>
     <t>Software Maintenance (Year 3)</t>
   </si>
   <si>
-    <t>Ongoing Labor (Year 3) ($50/man-hour)</t>
-  </si>
-  <si>
-    <t>Software Maintenance (Year 1)</t>
-  </si>
-  <si>
     <t>Assumptions:</t>
   </si>
   <si>
-    <t>Software maintenance is usually around 20% of original purchase cost</t>
-  </si>
-  <si>
     <t>"Ongoing Labor" would include things like creating new data models and tests, etc. Running the same tests on new versions of Firefox is not included in this estimate</t>
   </si>
   <si>
@@ -82,16 +68,40 @@
     <t>"Implementation - Labor" would include creating initial data models / tests for Firefox. Peach Professional comes with an existing set of "Peach Pits", which are the data models and tests made commercially available. I'm assuming Codenomican has something similar - and probably a wider variety</t>
   </si>
   <si>
-    <t>Purchase costs for Peach and Codenomicon are completely made up here. They have no price estimates on their sites, so I will email their sales contacts</t>
-  </si>
-  <si>
     <t>"Ease of use" for each product is captured in labor hours to build tests</t>
   </si>
   <si>
     <t xml:space="preserve"> </t>
   </si>
   <si>
-    <t>Google says the average Security Engineer makes a little under $90k/year, which works out to ~$43/hour. Our org uses $50/hour for the chargeback rate to projects for Security Engineer hours, so I went for the slightly higher number</t>
+    <t>$80,000+ (125)</t>
+  </si>
+  <si>
+    <t>$90,000+ (99)</t>
+  </si>
+  <si>
+    <t>$100,000+ (75)</t>
+  </si>
+  <si>
+    <t>$105,000+ (59)</t>
+  </si>
+  <si>
+    <t>$115,000+ (33)</t>
+  </si>
+  <si>
+    <t>Security Engineer Chargeback Rate</t>
+  </si>
+  <si>
+    <t>Glassdoor shows the average Security Engineer makes a little over $93k/year, which works out to ~$45/hour. This cost estimate can be programatically updated by changing the value in C24</t>
+  </si>
+  <si>
+    <t>Implementation - Labor ($45/man-hour)</t>
+  </si>
+  <si>
+    <t>Ongoing Labor (Year 2) ($45/man-hour)</t>
+  </si>
+  <si>
+    <t>Ongoing Labor (Year 3) ($45/man-hour)</t>
   </si>
 </sst>
 </file>
@@ -101,7 +111,7 @@
   <numFmts count="1">
     <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
   </numFmts>
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -147,6 +157,21 @@
       <name val="Calibri"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -165,34 +190,48 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="4">
+  <cellStyleXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1"/>
-    <xf numFmtId="44" fontId="2" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="2" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="44" fontId="7" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="7" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="44" fontId="6" fillId="0" borderId="0" xfId="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
-  <cellStyles count="4">
+  <cellStyles count="9">
     <cellStyle name="Currency" xfId="1" builtinId="4"/>
     <cellStyle name="Followed Hyperlink" xfId="3" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="5" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="7" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="8" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="2" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="4" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="6" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="9">
+  <dxfs count="12">
     <dxf>
       <font>
         <b val="0"/>
@@ -204,12 +243,37 @@
         <shadow val="0"/>
         <u val="none"/>
         <vertAlign val="baseline"/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <scheme val="minor"/>
-      </font>
-      <numFmt numFmtId="34" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
     </dxf>
     <dxf>
       <font>
@@ -222,7 +286,7 @@
         <shadow val="0"/>
         <u val="none"/>
         <vertAlign val="baseline"/>
-        <sz val="12"/>
+        <sz val="10"/>
         <color theme="1"/>
         <name val="Calibri"/>
         <scheme val="minor"/>
@@ -239,12 +303,11 @@
         <shadow val="0"/>
         <u val="none"/>
         <vertAlign val="baseline"/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <scheme val="minor"/>
-      </font>
-      <numFmt numFmtId="0" formatCode="General"/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
     </dxf>
     <dxf>
       <font>
@@ -257,7 +320,7 @@
         <shadow val="0"/>
         <u val="none"/>
         <vertAlign val="baseline"/>
-        <sz val="12"/>
+        <sz val="10"/>
         <color theme="1"/>
         <name val="Calibri"/>
         <scheme val="minor"/>
@@ -274,12 +337,24 @@
         <shadow val="0"/>
         <u val="none"/>
         <vertAlign val="baseline"/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <scheme val="minor"/>
-      </font>
-      <numFmt numFmtId="0" formatCode="General"/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
     </dxf>
     <dxf>
       <font>
@@ -297,6 +372,7 @@
         <name val="Calibri"/>
         <scheme val="minor"/>
       </font>
+      <numFmt numFmtId="34" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
     </dxf>
     <dxf>
       <font>
@@ -332,6 +408,7 @@
         <name val="Calibri"/>
         <scheme val="minor"/>
       </font>
+      <numFmt numFmtId="0" formatCode="General"/>
     </dxf>
     <dxf>
       <font>
@@ -349,6 +426,7 @@
         <name val="Calibri"/>
         <scheme val="minor"/>
       </font>
+      <numFmt numFmtId="0" formatCode="General"/>
     </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium7"/>
@@ -361,8 +439,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="B2:F11" dataDxfId="8" dataCellStyle="Currency">
-  <autoFilter ref="B2:F11">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="B2:F10" headerRowDxfId="2" dataDxfId="0" totalsRowDxfId="1" dataCellStyle="Currency">
+  <autoFilter ref="B2:F10">
     <filterColumn colId="0" hiddenButton="1"/>
     <filterColumn colId="1" hiddenButton="1"/>
     <filterColumn colId="2" hiddenButton="1"/>
@@ -370,11 +448,11 @@
     <filterColumn colId="4" hiddenButton="1"/>
   </autoFilter>
   <tableColumns count="5">
-    <tableColumn id="1" name=" " totalsRowLabel="Total"/>
-    <tableColumn id="2" name="Sulley" dataDxfId="7" totalsRowDxfId="6" dataCellStyle="Currency"/>
-    <tableColumn id="3" name="Peach_x000a_Community" dataDxfId="5" totalsRowDxfId="4" dataCellStyle="Currency"/>
-    <tableColumn id="4" name="Peach_x000a_Professional" dataDxfId="3" totalsRowDxfId="2" dataCellStyle="Currency"/>
-    <tableColumn id="5" name="Codenomicon" totalsRowFunction="sum" dataDxfId="1" totalsRowDxfId="0" dataCellStyle="Currency"/>
+    <tableColumn id="1" name=" " totalsRowLabel="Total" dataDxfId="7"/>
+    <tableColumn id="2" name="Sulley" dataDxfId="6" totalsRowDxfId="11" dataCellStyle="Currency"/>
+    <tableColumn id="3" name="Peach_x000a_Community" dataDxfId="5" totalsRowDxfId="10" dataCellStyle="Currency"/>
+    <tableColumn id="4" name="Peach_x000a_Professional" dataDxfId="4" totalsRowDxfId="9" dataCellStyle="Currency"/>
+    <tableColumn id="5" name="Codenomicon" totalsRowFunction="sum" dataDxfId="3" totalsRowDxfId="8" dataCellStyle="Currency"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium9" showFirstColumn="1" showLastColumn="0" showRowStripes="0" showColumnStripes="1"/>
 </table>
@@ -643,264 +721,341 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B2:G21"/>
+  <dimension ref="B2:G24"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="160" zoomScaleNormal="160" zoomScalePageLayoutView="160" workbookViewId="0">
-      <selection activeCell="F4" sqref="F4"/>
+      <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="4" customWidth="1"/>
-    <col min="2" max="2" width="34.33203125" customWidth="1"/>
-    <col min="3" max="6" width="14" style="1" customWidth="1"/>
+    <col min="2" max="2" width="28.83203125" customWidth="1"/>
+    <col min="3" max="3" width="9.5" style="1" customWidth="1"/>
+    <col min="4" max="4" width="9.33203125" style="1" customWidth="1"/>
+    <col min="5" max="5" width="10.5" style="1" customWidth="1"/>
+    <col min="6" max="6" width="11" style="1" customWidth="1"/>
+    <col min="8" max="8" width="7" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:7" ht="32" x14ac:dyDescent="0.2">
-      <c r="B2" t="s">
+    <row r="2" spans="2:7" ht="28" x14ac:dyDescent="0.2">
+      <c r="B2" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="C2" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="D2" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="E2" s="7" t="s">
+        <v>4</v>
+      </c>
+      <c r="F2" s="6" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B3" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="C3" s="8">
+        <v>0</v>
+      </c>
+      <c r="D3" s="8">
+        <v>0</v>
+      </c>
+      <c r="E3" s="8">
+        <v>21000</v>
+      </c>
+      <c r="F3" s="8">
+        <v>15000</v>
+      </c>
+    </row>
+    <row r="4" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B4" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="C4" s="8">
+        <f>200*C24</f>
+        <v>9000</v>
+      </c>
+      <c r="D4" s="8">
+        <f>300*C24</f>
+        <v>13500</v>
+      </c>
+      <c r="E4" s="8">
+        <f>80*C24</f>
+        <v>3600</v>
+      </c>
+      <c r="F4" s="8">
+        <f>80*C24</f>
+        <v>3600</v>
+      </c>
+    </row>
+    <row r="5" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B5" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="C5" s="8">
+        <v>0</v>
+      </c>
+      <c r="D5" s="8">
+        <v>0</v>
+      </c>
+      <c r="E5" s="8">
+        <v>21000</v>
+      </c>
+      <c r="F5" s="8">
+        <v>15000</v>
+      </c>
+    </row>
+    <row r="6" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B6" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="C6" s="8">
+        <f>75*C24</f>
+        <v>3375</v>
+      </c>
+      <c r="D6" s="8">
+        <f>150*C24</f>
+        <v>6750</v>
+      </c>
+      <c r="E6" s="8">
+        <f>40*C24</f>
+        <v>1800</v>
+      </c>
+      <c r="F6" s="8">
+        <f>40*C24</f>
+        <v>1800</v>
+      </c>
+    </row>
+    <row r="7" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B7" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="C7" s="8">
+        <v>0</v>
+      </c>
+      <c r="D7" s="8">
+        <v>0</v>
+      </c>
+      <c r="E7" s="8">
+        <f>E5</f>
+        <v>21000</v>
+      </c>
+      <c r="F7" s="8">
+        <f>F5</f>
+        <v>15000</v>
+      </c>
+    </row>
+    <row r="8" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B8" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="C8" s="8">
+        <f>75*C24</f>
+        <v>3375</v>
+      </c>
+      <c r="D8" s="8">
+        <f>150*C24</f>
+        <v>6750</v>
+      </c>
+      <c r="E8" s="8">
+        <f>40*C24</f>
+        <v>1800</v>
+      </c>
+      <c r="F8" s="8">
+        <f>40*C24</f>
+        <v>1800</v>
+      </c>
+    </row>
+    <row r="9" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B9" s="5"/>
+      <c r="C9" s="8"/>
+      <c r="D9" s="8"/>
+      <c r="E9" s="8"/>
+      <c r="F9" s="8"/>
+    </row>
+    <row r="10" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B10" s="9" t="s">
+        <v>2</v>
+      </c>
+      <c r="C10" s="8">
+        <f>SUM(C3:C9)</f>
+        <v>15750</v>
+      </c>
+      <c r="D10" s="8">
+        <f>SUM(D3:D9)</f>
+        <v>27000</v>
+      </c>
+      <c r="E10" s="8">
+        <f>SUM(E3:E9)</f>
+        <v>70200</v>
+      </c>
+      <c r="F10" s="8">
+        <f>SUM(F3:F9)</f>
+        <v>52200</v>
+      </c>
+    </row>
+    <row r="11" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="C11"/>
+      <c r="D11"/>
+      <c r="E11"/>
+      <c r="F11"/>
+    </row>
+    <row r="13" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B13" s="3" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="14" spans="2:7" ht="41" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B14" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="C14" s="4"/>
+      <c r="D14" s="4"/>
+      <c r="E14" s="4"/>
+      <c r="F14" s="4"/>
+      <c r="G14" s="4"/>
+    </row>
+    <row r="16" spans="2:7" ht="65" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B16" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="C16" s="4"/>
+      <c r="D16" s="4"/>
+      <c r="E16" s="4"/>
+      <c r="F16" s="4"/>
+      <c r="G16" s="4"/>
+    </row>
+    <row r="17" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="B17" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="18" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="B18" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="19" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="B19" s="2"/>
+    </row>
+    <row r="20" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="B20" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="24" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="B24" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="C2" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="D2" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="E2" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="F2" s="2" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="3" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B3" t="s">
-        <v>6</v>
-      </c>
-      <c r="C3" s="1">
-        <v>0</v>
-      </c>
-      <c r="D3" s="1">
-        <v>0</v>
-      </c>
-      <c r="E3" s="1">
-        <v>5000</v>
-      </c>
-      <c r="F3" s="1">
-        <v>15000</v>
-      </c>
-    </row>
-    <row r="4" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B4" t="s">
-        <v>2</v>
-      </c>
-      <c r="C4" s="1">
-        <f>200*50</f>
-        <v>10000</v>
-      </c>
-      <c r="D4" s="1">
-        <f>200*50</f>
-        <v>10000</v>
-      </c>
-      <c r="E4" s="1">
-        <f>100*50</f>
-        <v>5000</v>
-      </c>
-      <c r="F4" s="1">
-        <f>80*50</f>
-        <v>4000</v>
-      </c>
-    </row>
-    <row r="5" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B5" t="s">
-        <v>11</v>
-      </c>
-      <c r="C5" s="1">
-        <f>C3*0.2</f>
-        <v>0</v>
-      </c>
-      <c r="D5" s="1">
-        <f>D3*0.2</f>
-        <v>0</v>
-      </c>
-      <c r="E5" s="1">
-        <f>E3*0.2</f>
-        <v>1000</v>
-      </c>
-      <c r="F5" s="1">
-        <f>F3*0.2</f>
-        <v>3000</v>
-      </c>
-    </row>
-    <row r="6" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B6" t="s">
-        <v>8</v>
-      </c>
-      <c r="C6" s="1">
-        <f>C5</f>
-        <v>0</v>
-      </c>
-      <c r="D6" s="1">
-        <f t="shared" ref="D6:F6" si="0">D5</f>
-        <v>0</v>
-      </c>
-      <c r="E6" s="1">
-        <f t="shared" si="0"/>
-        <v>1000</v>
-      </c>
-      <c r="F6" s="1">
-        <f t="shared" si="0"/>
-        <v>3000</v>
-      </c>
-    </row>
-    <row r="7" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B7" t="s">
-        <v>7</v>
-      </c>
-      <c r="C7" s="1">
-        <f>100*50</f>
-        <v>5000</v>
-      </c>
-      <c r="D7" s="1">
-        <f>100*50</f>
-        <v>5000</v>
-      </c>
-      <c r="E7" s="1">
-        <f>50*50</f>
-        <v>2500</v>
-      </c>
-      <c r="F7" s="1">
-        <f>40*50</f>
-        <v>2000</v>
-      </c>
-    </row>
-    <row r="8" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B8" t="s">
-        <v>9</v>
-      </c>
-      <c r="C8" s="1">
-        <f>C5</f>
-        <v>0</v>
-      </c>
-      <c r="D8" s="1">
-        <f t="shared" ref="D8:F8" si="1">D5</f>
-        <v>0</v>
-      </c>
-      <c r="E8" s="1">
-        <f t="shared" si="1"/>
-        <v>1000</v>
-      </c>
-      <c r="F8" s="1">
-        <f t="shared" si="1"/>
-        <v>3000</v>
-      </c>
-    </row>
-    <row r="9" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B9" t="s">
-        <v>10</v>
-      </c>
-      <c r="C9" s="1">
-        <f>100*50</f>
-        <v>5000</v>
-      </c>
-      <c r="D9" s="1">
-        <f>100*50</f>
-        <v>5000</v>
-      </c>
-      <c r="E9" s="1">
-        <f>40*50</f>
-        <v>2000</v>
-      </c>
-      <c r="F9" s="1">
-        <f>25*50</f>
-        <v>1250</v>
-      </c>
-    </row>
-    <row r="11" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B11" s="5" t="s">
-        <v>3</v>
-      </c>
-      <c r="C11" s="1">
-        <f>SUM(C3:C10)</f>
-        <v>20000</v>
-      </c>
-      <c r="D11" s="1">
-        <f>SUM(D3:D10)</f>
-        <v>20000</v>
-      </c>
-      <c r="E11" s="1">
-        <f>SUM(E3:E10)</f>
-        <v>17500</v>
-      </c>
-      <c r="F11" s="1">
-        <f>SUM(F3:F10)</f>
-        <v>31250</v>
-      </c>
-    </row>
-    <row r="12" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="C12"/>
-      <c r="D12"/>
-      <c r="E12"/>
-      <c r="F12"/>
-    </row>
-    <row r="14" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B14" s="5" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="15" spans="2:7" ht="35" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B15" s="6" t="s">
-        <v>20</v>
-      </c>
-      <c r="C15" s="6"/>
-      <c r="D15" s="6"/>
-      <c r="E15" s="6"/>
-      <c r="F15" s="6"/>
-      <c r="G15" s="6"/>
-    </row>
-    <row r="16" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B16" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="17" spans="2:7" ht="49" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B17" s="6" t="s">
-        <v>16</v>
-      </c>
-      <c r="C17" s="6"/>
-      <c r="D17" s="6"/>
-      <c r="E17" s="6"/>
-      <c r="F17" s="6"/>
-      <c r="G17" s="6"/>
-    </row>
-    <row r="18" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B18" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="19" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B19" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="20" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B20" s="4" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="21" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B21" t="s">
-        <v>18</v>
+      <c r="C24" s="1">
+        <v>45</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="2">
-    <mergeCell ref="B17:G17"/>
-    <mergeCell ref="B15:G15"/>
+    <mergeCell ref="B16:G16"/>
+    <mergeCell ref="B14:G14"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <ignoredErrors>
+    <ignoredError sqref="E7" formula="1"/>
+  </ignoredErrors>
   <tableParts count="1">
     <tablePart r:id="rId1"/>
   </tableParts>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:G17"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G13" sqref="G13"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="13.33203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.5" style="1" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="11.33203125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="D13" s="1">
+        <v>80000</v>
+      </c>
+      <c r="E13">
+        <v>125</v>
+      </c>
+      <c r="G13" s="10">
+        <f>SUMPRODUCT(D13:D17,E13:E17)/SUM(E13:E17)</f>
+        <v>93094.629156010225</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="D14" s="1">
+        <v>90000</v>
+      </c>
+      <c r="E14">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="D15" s="1">
+        <v>100000</v>
+      </c>
+      <c r="E15">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="D16" s="1">
+        <v>105000</v>
+      </c>
+      <c r="E16">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="17" spans="4:5" x14ac:dyDescent="0.2">
+      <c r="D17" s="1">
+        <v>115000</v>
+      </c>
+      <c r="E17">
+        <v>33</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>